<commit_message>
Phylogenetic tree with filtered 609 E. coli targets colored by phyla
</commit_message>
<xml_diff>
--- a/Manuscript/Pipeline_results_summary.xlsx
+++ b/Manuscript/Pipeline_results_summary.xlsx
@@ -624,7 +624,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -842,6 +842,9 @@
       <c r="G14" s="1">
         <v>2184</v>
       </c>
+      <c r="K14" s="1">
+        <v>1293</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="C16" s="1" t="s">

</xml_diff>